<commit_message>
✅ Fix: claves 'Corners' y 'Tarjetas' corregidas en promedios
</commit_message>
<xml_diff>
--- a/Ligas/Liga_Suecia_2025.xlsx
+++ b/Ligas/Liga_Suecia_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A24006-3D90-40E9-AC6F-5BA2BF1550F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF67B25-FFD5-4FD4-91EE-256C50536D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -648,13 +648,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="Q118" sqref="Q1:R1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Actualizar fixtures de todas las ligas (goles por tiempo, stats) 2025-08-15
</commit_message>
<xml_diff>
--- a/Ligas/Liga_Suecia_2025.xlsx
+++ b/Ligas/Liga_Suecia_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U145"/>
+  <dimension ref="A1:Y153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,6 +539,26 @@
           <t>Posesión Visita ().1</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Posesión Local (%)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Posesión Visita (%)</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>fuente_tiempos</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>estado_datos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -608,6 +628,10 @@
       </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -677,6 +701,10 @@
       </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -746,6 +774,10 @@
       </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -815,6 +847,10 @@
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -884,6 +920,10 @@
       </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -953,6 +993,10 @@
       </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1022,6 +1066,10 @@
       </c>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1091,6 +1139,10 @@
       </c>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1160,6 +1212,10 @@
       </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1229,6 +1285,10 @@
       </c>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1298,6 +1358,10 @@
       </c>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1367,6 +1431,10 @@
       </c>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1436,6 +1504,10 @@
       </c>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1505,6 +1577,10 @@
       </c>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1574,6 +1650,10 @@
       </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1643,6 +1723,10 @@
       </c>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1712,6 +1796,10 @@
       </c>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1781,6 +1869,10 @@
       </c>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1850,6 +1942,10 @@
       </c>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1919,6 +2015,10 @@
       </c>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1988,6 +2088,10 @@
       </c>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2057,6 +2161,10 @@
       </c>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2126,6 +2234,10 @@
       </c>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2195,6 +2307,10 @@
       </c>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2264,6 +2380,10 @@
       </c>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2333,6 +2453,10 @@
       </c>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2402,6 +2526,10 @@
       </c>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2471,6 +2599,10 @@
       </c>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2540,6 +2672,10 @@
       </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2609,6 +2745,10 @@
       </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2678,6 +2818,10 @@
       </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2747,6 +2891,10 @@
       </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2816,6 +2964,10 @@
       </c>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2885,6 +3037,10 @@
       </c>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2954,6 +3110,10 @@
       </c>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
+      <c r="X36" t="inlineStr"/>
+      <c r="Y36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3023,6 +3183,10 @@
       </c>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
+      <c r="Y37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3092,6 +3256,10 @@
       </c>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
+      <c r="X38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3161,6 +3329,10 @@
       </c>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3230,6 +3402,10 @@
       </c>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3299,6 +3475,10 @@
       </c>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3368,6 +3548,10 @@
       </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr"/>
+      <c r="Y42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3437,6 +3621,10 @@
       </c>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3506,6 +3694,10 @@
       </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr"/>
+      <c r="Y44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3575,6 +3767,10 @@
       </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr"/>
+      <c r="Y45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3644,6 +3840,10 @@
       </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3713,6 +3913,10 @@
       </c>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr"/>
+      <c r="Y47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3782,6 +3986,10 @@
       </c>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3851,6 +4059,10 @@
       </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3920,6 +4132,10 @@
       </c>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3989,6 +4205,10 @@
       </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4058,6 +4278,10 @@
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4127,6 +4351,10 @@
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4196,6 +4424,10 @@
       </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4265,6 +4497,10 @@
       </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4334,6 +4570,10 @@
       </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4403,6 +4643,10 @@
       </c>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4472,6 +4716,10 @@
       </c>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+      <c r="Y58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4541,6 +4789,10 @@
       </c>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+      <c r="Y59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4610,6 +4862,10 @@
       </c>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr"/>
+      <c r="Y60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4679,6 +4935,10 @@
       </c>
       <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr"/>
+      <c r="Y61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4748,6 +5008,10 @@
       </c>
       <c r="T62" t="inlineStr"/>
       <c r="U62" t="inlineStr"/>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr"/>
+      <c r="Y62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4817,6 +5081,10 @@
       </c>
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr"/>
+      <c r="V63" t="inlineStr"/>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr"/>
+      <c r="Y63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4886,6 +5154,10 @@
       </c>
       <c r="T64" t="inlineStr"/>
       <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
+      <c r="Y64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4955,6 +5227,10 @@
       </c>
       <c r="T65" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
+      <c r="V65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr"/>
+      <c r="Y65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -5024,6 +5300,10 @@
       </c>
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
+      <c r="V66" t="inlineStr"/>
+      <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr"/>
+      <c r="Y66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5093,6 +5373,10 @@
       </c>
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
+      <c r="V67" t="inlineStr"/>
+      <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr"/>
+      <c r="Y67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5162,6 +5446,10 @@
       </c>
       <c r="T68" t="inlineStr"/>
       <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr"/>
+      <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr"/>
+      <c r="Y68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5231,6 +5519,10 @@
       </c>
       <c r="T69" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
+      <c r="V69" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr"/>
+      <c r="Y69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5300,6 +5592,10 @@
       </c>
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
+      <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr"/>
+      <c r="Y70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5369,6 +5665,10 @@
       </c>
       <c r="T71" t="inlineStr"/>
       <c r="U71" t="inlineStr"/>
+      <c r="V71" t="inlineStr"/>
+      <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr"/>
+      <c r="Y71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -5438,6 +5738,10 @@
       </c>
       <c r="T72" t="inlineStr"/>
       <c r="U72" t="inlineStr"/>
+      <c r="V72" t="inlineStr"/>
+      <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr"/>
+      <c r="Y72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5507,6 +5811,10 @@
       </c>
       <c r="T73" t="inlineStr"/>
       <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr"/>
+      <c r="Y73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5576,6 +5884,10 @@
       </c>
       <c r="T74" t="inlineStr"/>
       <c r="U74" t="inlineStr"/>
+      <c r="V74" t="inlineStr"/>
+      <c r="W74" t="inlineStr"/>
+      <c r="X74" t="inlineStr"/>
+      <c r="Y74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -5645,6 +5957,10 @@
       </c>
       <c r="T75" t="inlineStr"/>
       <c r="U75" t="inlineStr"/>
+      <c r="V75" t="inlineStr"/>
+      <c r="W75" t="inlineStr"/>
+      <c r="X75" t="inlineStr"/>
+      <c r="Y75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -5714,6 +6030,10 @@
       </c>
       <c r="T76" t="inlineStr"/>
       <c r="U76" t="inlineStr"/>
+      <c r="V76" t="inlineStr"/>
+      <c r="W76" t="inlineStr"/>
+      <c r="X76" t="inlineStr"/>
+      <c r="Y76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -5783,6 +6103,10 @@
       </c>
       <c r="T77" t="inlineStr"/>
       <c r="U77" t="inlineStr"/>
+      <c r="V77" t="inlineStr"/>
+      <c r="W77" t="inlineStr"/>
+      <c r="X77" t="inlineStr"/>
+      <c r="Y77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -5852,6 +6176,10 @@
       </c>
       <c r="T78" t="inlineStr"/>
       <c r="U78" t="inlineStr"/>
+      <c r="V78" t="inlineStr"/>
+      <c r="W78" t="inlineStr"/>
+      <c r="X78" t="inlineStr"/>
+      <c r="Y78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -5921,6 +6249,10 @@
       </c>
       <c r="T79" t="inlineStr"/>
       <c r="U79" t="inlineStr"/>
+      <c r="V79" t="inlineStr"/>
+      <c r="W79" t="inlineStr"/>
+      <c r="X79" t="inlineStr"/>
+      <c r="Y79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -5990,6 +6322,10 @@
       </c>
       <c r="T80" t="inlineStr"/>
       <c r="U80" t="inlineStr"/>
+      <c r="V80" t="inlineStr"/>
+      <c r="W80" t="inlineStr"/>
+      <c r="X80" t="inlineStr"/>
+      <c r="Y80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -6059,6 +6395,10 @@
       </c>
       <c r="T81" t="inlineStr"/>
       <c r="U81" t="inlineStr"/>
+      <c r="V81" t="inlineStr"/>
+      <c r="W81" t="inlineStr"/>
+      <c r="X81" t="inlineStr"/>
+      <c r="Y81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -6128,6 +6468,10 @@
       </c>
       <c r="T82" t="inlineStr"/>
       <c r="U82" t="inlineStr"/>
+      <c r="V82" t="inlineStr"/>
+      <c r="W82" t="inlineStr"/>
+      <c r="X82" t="inlineStr"/>
+      <c r="Y82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -6197,6 +6541,10 @@
       </c>
       <c r="T83" t="inlineStr"/>
       <c r="U83" t="inlineStr"/>
+      <c r="V83" t="inlineStr"/>
+      <c r="W83" t="inlineStr"/>
+      <c r="X83" t="inlineStr"/>
+      <c r="Y83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -6266,6 +6614,10 @@
       </c>
       <c r="T84" t="inlineStr"/>
       <c r="U84" t="inlineStr"/>
+      <c r="V84" t="inlineStr"/>
+      <c r="W84" t="inlineStr"/>
+      <c r="X84" t="inlineStr"/>
+      <c r="Y84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -6335,6 +6687,10 @@
       </c>
       <c r="T85" t="inlineStr"/>
       <c r="U85" t="inlineStr"/>
+      <c r="V85" t="inlineStr"/>
+      <c r="W85" t="inlineStr"/>
+      <c r="X85" t="inlineStr"/>
+      <c r="Y85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -6404,6 +6760,10 @@
       </c>
       <c r="T86" t="inlineStr"/>
       <c r="U86" t="inlineStr"/>
+      <c r="V86" t="inlineStr"/>
+      <c r="W86" t="inlineStr"/>
+      <c r="X86" t="inlineStr"/>
+      <c r="Y86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -6473,6 +6833,10 @@
       </c>
       <c r="T87" t="inlineStr"/>
       <c r="U87" t="inlineStr"/>
+      <c r="V87" t="inlineStr"/>
+      <c r="W87" t="inlineStr"/>
+      <c r="X87" t="inlineStr"/>
+      <c r="Y87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -6542,6 +6906,10 @@
       </c>
       <c r="T88" t="inlineStr"/>
       <c r="U88" t="inlineStr"/>
+      <c r="V88" t="inlineStr"/>
+      <c r="W88" t="inlineStr"/>
+      <c r="X88" t="inlineStr"/>
+      <c r="Y88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6611,6 +6979,10 @@
       </c>
       <c r="T89" t="inlineStr"/>
       <c r="U89" t="inlineStr"/>
+      <c r="V89" t="inlineStr"/>
+      <c r="W89" t="inlineStr"/>
+      <c r="X89" t="inlineStr"/>
+      <c r="Y89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -6680,6 +7052,10 @@
       </c>
       <c r="T90" t="inlineStr"/>
       <c r="U90" t="inlineStr"/>
+      <c r="V90" t="inlineStr"/>
+      <c r="W90" t="inlineStr"/>
+      <c r="X90" t="inlineStr"/>
+      <c r="Y90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -6749,6 +7125,10 @@
       </c>
       <c r="T91" t="inlineStr"/>
       <c r="U91" t="inlineStr"/>
+      <c r="V91" t="inlineStr"/>
+      <c r="W91" t="inlineStr"/>
+      <c r="X91" t="inlineStr"/>
+      <c r="Y91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -6818,6 +7198,10 @@
       </c>
       <c r="T92" t="inlineStr"/>
       <c r="U92" t="inlineStr"/>
+      <c r="V92" t="inlineStr"/>
+      <c r="W92" t="inlineStr"/>
+      <c r="X92" t="inlineStr"/>
+      <c r="Y92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -6887,6 +7271,10 @@
       </c>
       <c r="T93" t="inlineStr"/>
       <c r="U93" t="inlineStr"/>
+      <c r="V93" t="inlineStr"/>
+      <c r="W93" t="inlineStr"/>
+      <c r="X93" t="inlineStr"/>
+      <c r="Y93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -6956,6 +7344,10 @@
       </c>
       <c r="T94" t="inlineStr"/>
       <c r="U94" t="inlineStr"/>
+      <c r="V94" t="inlineStr"/>
+      <c r="W94" t="inlineStr"/>
+      <c r="X94" t="inlineStr"/>
+      <c r="Y94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -7025,6 +7417,10 @@
       </c>
       <c r="T95" t="inlineStr"/>
       <c r="U95" t="inlineStr"/>
+      <c r="V95" t="inlineStr"/>
+      <c r="W95" t="inlineStr"/>
+      <c r="X95" t="inlineStr"/>
+      <c r="Y95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -7094,6 +7490,10 @@
       </c>
       <c r="T96" t="inlineStr"/>
       <c r="U96" t="inlineStr"/>
+      <c r="V96" t="inlineStr"/>
+      <c r="W96" t="inlineStr"/>
+      <c r="X96" t="inlineStr"/>
+      <c r="Y96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -7163,6 +7563,10 @@
       </c>
       <c r="T97" t="inlineStr"/>
       <c r="U97" t="inlineStr"/>
+      <c r="V97" t="inlineStr"/>
+      <c r="W97" t="inlineStr"/>
+      <c r="X97" t="inlineStr"/>
+      <c r="Y97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -7232,6 +7636,10 @@
       </c>
       <c r="T98" t="inlineStr"/>
       <c r="U98" t="inlineStr"/>
+      <c r="V98" t="inlineStr"/>
+      <c r="W98" t="inlineStr"/>
+      <c r="X98" t="inlineStr"/>
+      <c r="Y98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -7301,6 +7709,10 @@
       </c>
       <c r="T99" t="inlineStr"/>
       <c r="U99" t="inlineStr"/>
+      <c r="V99" t="inlineStr"/>
+      <c r="W99" t="inlineStr"/>
+      <c r="X99" t="inlineStr"/>
+      <c r="Y99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -7370,6 +7782,10 @@
       </c>
       <c r="T100" t="inlineStr"/>
       <c r="U100" t="inlineStr"/>
+      <c r="V100" t="inlineStr"/>
+      <c r="W100" t="inlineStr"/>
+      <c r="X100" t="inlineStr"/>
+      <c r="Y100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -7439,6 +7855,10 @@
       </c>
       <c r="T101" t="inlineStr"/>
       <c r="U101" t="inlineStr"/>
+      <c r="V101" t="inlineStr"/>
+      <c r="W101" t="inlineStr"/>
+      <c r="X101" t="inlineStr"/>
+      <c r="Y101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -7508,6 +7928,10 @@
       </c>
       <c r="T102" t="inlineStr"/>
       <c r="U102" t="inlineStr"/>
+      <c r="V102" t="inlineStr"/>
+      <c r="W102" t="inlineStr"/>
+      <c r="X102" t="inlineStr"/>
+      <c r="Y102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -7577,6 +8001,10 @@
       </c>
       <c r="T103" t="inlineStr"/>
       <c r="U103" t="inlineStr"/>
+      <c r="V103" t="inlineStr"/>
+      <c r="W103" t="inlineStr"/>
+      <c r="X103" t="inlineStr"/>
+      <c r="Y103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -7646,6 +8074,10 @@
       </c>
       <c r="T104" t="inlineStr"/>
       <c r="U104" t="inlineStr"/>
+      <c r="V104" t="inlineStr"/>
+      <c r="W104" t="inlineStr"/>
+      <c r="X104" t="inlineStr"/>
+      <c r="Y104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -7715,6 +8147,10 @@
       </c>
       <c r="T105" t="inlineStr"/>
       <c r="U105" t="inlineStr"/>
+      <c r="V105" t="inlineStr"/>
+      <c r="W105" t="inlineStr"/>
+      <c r="X105" t="inlineStr"/>
+      <c r="Y105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -7784,6 +8220,10 @@
       </c>
       <c r="T106" t="inlineStr"/>
       <c r="U106" t="inlineStr"/>
+      <c r="V106" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
+      <c r="X106" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -7853,6 +8293,10 @@
       </c>
       <c r="T107" t="inlineStr"/>
       <c r="U107" t="inlineStr"/>
+      <c r="V107" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
+      <c r="X107" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -7922,6 +8366,10 @@
       </c>
       <c r="T108" t="inlineStr"/>
       <c r="U108" t="inlineStr"/>
+      <c r="V108" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
+      <c r="X108" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -7991,6 +8439,10 @@
       </c>
       <c r="T109" t="inlineStr"/>
       <c r="U109" t="inlineStr"/>
+      <c r="V109" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -8060,6 +8512,10 @@
       </c>
       <c r="T110" t="inlineStr"/>
       <c r="U110" t="inlineStr"/>
+      <c r="V110" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
+      <c r="X110" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -8129,6 +8585,10 @@
       </c>
       <c r="T111" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
+      <c r="V111" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
+      <c r="X111" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -8198,6 +8658,10 @@
       </c>
       <c r="T112" t="inlineStr"/>
       <c r="U112" t="inlineStr"/>
+      <c r="V112" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
+      <c r="X112" t="inlineStr"/>
+      <c r="Y112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -8267,6 +8731,10 @@
       </c>
       <c r="T113" t="inlineStr"/>
       <c r="U113" t="inlineStr"/>
+      <c r="V113" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
+      <c r="X113" t="inlineStr"/>
+      <c r="Y113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -8336,6 +8804,10 @@
       </c>
       <c r="T114" t="inlineStr"/>
       <c r="U114" t="inlineStr"/>
+      <c r="V114" t="inlineStr"/>
+      <c r="W114" t="inlineStr"/>
+      <c r="X114" t="inlineStr"/>
+      <c r="Y114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -8405,6 +8877,10 @@
       </c>
       <c r="T115" t="inlineStr"/>
       <c r="U115" t="inlineStr"/>
+      <c r="V115" t="inlineStr"/>
+      <c r="W115" t="inlineStr"/>
+      <c r="X115" t="inlineStr"/>
+      <c r="Y115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -8474,6 +8950,10 @@
       </c>
       <c r="T116" t="inlineStr"/>
       <c r="U116" t="inlineStr"/>
+      <c r="V116" t="inlineStr"/>
+      <c r="W116" t="inlineStr"/>
+      <c r="X116" t="inlineStr"/>
+      <c r="Y116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -8531,10 +9011,10 @@
         <v>1</v>
       </c>
       <c r="Q117" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R117" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S117" t="inlineStr">
         <is>
@@ -8543,6 +9023,10 @@
       </c>
       <c r="T117" t="inlineStr"/>
       <c r="U117" t="inlineStr"/>
+      <c r="V117" t="inlineStr"/>
+      <c r="W117" t="inlineStr"/>
+      <c r="X117" t="inlineStr"/>
+      <c r="Y117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -8612,6 +9096,10 @@
       </c>
       <c r="T118" t="inlineStr"/>
       <c r="U118" t="inlineStr"/>
+      <c r="V118" t="inlineStr"/>
+      <c r="W118" t="inlineStr"/>
+      <c r="X118" t="inlineStr"/>
+      <c r="Y118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -8657,13 +9145,13 @@
         <v>0</v>
       </c>
       <c r="M119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N119" t="n">
         <v>0</v>
       </c>
       <c r="O119" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P119" t="n">
         <v>2</v>
@@ -8681,6 +9169,10 @@
       </c>
       <c r="T119" t="inlineStr"/>
       <c r="U119" t="inlineStr"/>
+      <c r="V119" t="inlineStr"/>
+      <c r="W119" t="inlineStr"/>
+      <c r="X119" t="inlineStr"/>
+      <c r="Y119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -8726,13 +9218,13 @@
         <v>0</v>
       </c>
       <c r="M120" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N120" t="n">
         <v>0</v>
       </c>
       <c r="O120" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P120" t="n">
         <v>0</v>
@@ -8750,6 +9242,10 @@
       </c>
       <c r="T120" t="inlineStr"/>
       <c r="U120" t="inlineStr"/>
+      <c r="V120" t="inlineStr"/>
+      <c r="W120" t="inlineStr"/>
+      <c r="X120" t="inlineStr"/>
+      <c r="Y120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -8819,6 +9315,10 @@
       </c>
       <c r="T121" t="inlineStr"/>
       <c r="U121" t="inlineStr"/>
+      <c r="V121" t="inlineStr"/>
+      <c r="W121" t="inlineStr"/>
+      <c r="X121" t="inlineStr"/>
+      <c r="Y121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -8864,13 +9364,13 @@
         <v>0</v>
       </c>
       <c r="M122" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N122" t="n">
         <v>0</v>
       </c>
       <c r="O122" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P122" t="n">
         <v>1</v>
@@ -8888,6 +9388,10 @@
       </c>
       <c r="T122" t="inlineStr"/>
       <c r="U122" t="inlineStr"/>
+      <c r="V122" t="inlineStr"/>
+      <c r="W122" t="inlineStr"/>
+      <c r="X122" t="inlineStr"/>
+      <c r="Y122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -8936,13 +9440,13 @@
         <v>0</v>
       </c>
       <c r="N123" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O123" t="n">
         <v>1</v>
       </c>
       <c r="P123" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q123" t="n">
         <v>53</v>
@@ -8957,6 +9461,10 @@
       </c>
       <c r="T123" t="inlineStr"/>
       <c r="U123" t="inlineStr"/>
+      <c r="V123" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
+      <c r="X123" t="inlineStr"/>
+      <c r="Y123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -9002,13 +9510,13 @@
         <v>0</v>
       </c>
       <c r="M124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N124" t="n">
         <v>0</v>
       </c>
       <c r="O124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P124" t="n">
         <v>0</v>
@@ -9026,6 +9534,10 @@
       </c>
       <c r="T124" t="inlineStr"/>
       <c r="U124" t="inlineStr"/>
+      <c r="V124" t="inlineStr"/>
+      <c r="W124" t="inlineStr"/>
+      <c r="X124" t="inlineStr"/>
+      <c r="Y124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -9074,13 +9586,13 @@
         <v>0</v>
       </c>
       <c r="N125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O125" t="n">
         <v>0</v>
       </c>
       <c r="P125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q125" t="n">
         <v>37</v>
@@ -9095,6 +9607,10 @@
       </c>
       <c r="T125" t="inlineStr"/>
       <c r="U125" t="inlineStr"/>
+      <c r="V125" t="inlineStr"/>
+      <c r="W125" t="inlineStr"/>
+      <c r="X125" t="inlineStr"/>
+      <c r="Y125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -9143,13 +9659,13 @@
         <v>0</v>
       </c>
       <c r="N126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O126" t="n">
         <v>0</v>
       </c>
       <c r="P126" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q126" t="n">
         <v>53</v>
@@ -9164,6 +9680,10 @@
       </c>
       <c r="T126" t="inlineStr"/>
       <c r="U126" t="inlineStr"/>
+      <c r="V126" t="inlineStr"/>
+      <c r="W126" t="inlineStr"/>
+      <c r="X126" t="inlineStr"/>
+      <c r="Y126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -9233,6 +9753,10 @@
       </c>
       <c r="T127" t="inlineStr"/>
       <c r="U127" t="inlineStr"/>
+      <c r="V127" t="inlineStr"/>
+      <c r="W127" t="inlineStr"/>
+      <c r="X127" t="inlineStr"/>
+      <c r="Y127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -9302,6 +9826,10 @@
       </c>
       <c r="T128" t="inlineStr"/>
       <c r="U128" t="inlineStr"/>
+      <c r="V128" t="inlineStr"/>
+      <c r="W128" t="inlineStr"/>
+      <c r="X128" t="inlineStr"/>
+      <c r="Y128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -9350,13 +9878,13 @@
         <v>0</v>
       </c>
       <c r="N129" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O129" t="n">
         <v>3</v>
       </c>
       <c r="P129" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q129" t="n">
         <v>70</v>
@@ -9371,6 +9899,10 @@
       </c>
       <c r="T129" t="inlineStr"/>
       <c r="U129" t="inlineStr"/>
+      <c r="V129" t="inlineStr"/>
+      <c r="W129" t="inlineStr"/>
+      <c r="X129" t="inlineStr"/>
+      <c r="Y129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -9428,10 +9960,10 @@
         <v>0</v>
       </c>
       <c r="Q130" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R130" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S130" t="inlineStr">
         <is>
@@ -9440,6 +9972,10 @@
       </c>
       <c r="T130" t="inlineStr"/>
       <c r="U130" t="inlineStr"/>
+      <c r="V130" t="inlineStr"/>
+      <c r="W130" t="inlineStr"/>
+      <c r="X130" t="inlineStr"/>
+      <c r="Y130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -9485,13 +10021,13 @@
         <v>0</v>
       </c>
       <c r="M131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N131" t="n">
         <v>0</v>
       </c>
       <c r="O131" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P131" t="n">
         <v>1</v>
@@ -9509,6 +10045,10 @@
       </c>
       <c r="T131" t="inlineStr"/>
       <c r="U131" t="inlineStr"/>
+      <c r="V131" t="inlineStr"/>
+      <c r="W131" t="inlineStr"/>
+      <c r="X131" t="inlineStr"/>
+      <c r="Y131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -9554,16 +10094,16 @@
         <v>0</v>
       </c>
       <c r="M132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O132" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P132" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q132" t="n">
         <v>32</v>
@@ -9578,6 +10118,10 @@
       </c>
       <c r="T132" t="inlineStr"/>
       <c r="U132" t="inlineStr"/>
+      <c r="V132" t="inlineStr"/>
+      <c r="W132" t="inlineStr"/>
+      <c r="X132" t="inlineStr"/>
+      <c r="Y132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -9623,13 +10167,13 @@
         <v>0</v>
       </c>
       <c r="M133" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N133" t="n">
         <v>0</v>
       </c>
       <c r="O133" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P133" t="n">
         <v>0</v>
@@ -9647,6 +10191,10 @@
       </c>
       <c r="T133" t="inlineStr"/>
       <c r="U133" t="inlineStr"/>
+      <c r="V133" t="inlineStr"/>
+      <c r="W133" t="inlineStr"/>
+      <c r="X133" t="inlineStr"/>
+      <c r="Y133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -9716,6 +10264,10 @@
       </c>
       <c r="T134" t="inlineStr"/>
       <c r="U134" t="inlineStr"/>
+      <c r="V134" t="inlineStr"/>
+      <c r="W134" t="inlineStr"/>
+      <c r="X134" t="inlineStr"/>
+      <c r="Y134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -9764,13 +10316,13 @@
         <v>0</v>
       </c>
       <c r="N135" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O135" t="n">
         <v>1</v>
       </c>
       <c r="P135" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Q135" t="n">
         <v>49</v>
@@ -9785,6 +10337,10 @@
       </c>
       <c r="T135" t="inlineStr"/>
       <c r="U135" t="inlineStr"/>
+      <c r="V135" t="inlineStr"/>
+      <c r="W135" t="inlineStr"/>
+      <c r="X135" t="inlineStr"/>
+      <c r="Y135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -9854,6 +10410,10 @@
       </c>
       <c r="T136" t="inlineStr"/>
       <c r="U136" t="inlineStr"/>
+      <c r="V136" t="inlineStr"/>
+      <c r="W136" t="inlineStr"/>
+      <c r="X136" t="inlineStr"/>
+      <c r="Y136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -9887,10 +10447,10 @@
         <v>6</v>
       </c>
       <c r="I137" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K137" t="n">
         <v>0</v>
@@ -9899,16 +10459,16 @@
         <v>0</v>
       </c>
       <c r="M137" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O137" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P137" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q137" t="n">
         <v>34</v>
@@ -9923,6 +10483,10 @@
       </c>
       <c r="T137" t="inlineStr"/>
       <c r="U137" t="inlineStr"/>
+      <c r="V137" t="inlineStr"/>
+      <c r="W137" t="inlineStr"/>
+      <c r="X137" t="inlineStr"/>
+      <c r="Y137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -9955,12 +10519,8 @@
       <c r="H138" t="n">
         <v>2</v>
       </c>
-      <c r="I138" t="n">
-        <v>0</v>
-      </c>
-      <c r="J138" t="n">
-        <v>0</v>
-      </c>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" t="inlineStr"/>
       <c r="K138" t="n">
         <v>0</v>
       </c>
@@ -9971,13 +10531,13 @@
         <v>0</v>
       </c>
       <c r="N138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O138" t="n">
         <v>2</v>
       </c>
       <c r="P138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q138" t="n">
         <v>57</v>
@@ -9992,6 +10552,10 @@
       </c>
       <c r="T138" t="inlineStr"/>
       <c r="U138" t="inlineStr"/>
+      <c r="V138" t="inlineStr"/>
+      <c r="W138" t="inlineStr"/>
+      <c r="X138" t="inlineStr"/>
+      <c r="Y138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -10037,16 +10601,16 @@
         <v>0</v>
       </c>
       <c r="M139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N139" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O139" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P139" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q139" t="n">
         <v>58</v>
@@ -10061,6 +10625,10 @@
       </c>
       <c r="T139" t="inlineStr"/>
       <c r="U139" t="inlineStr"/>
+      <c r="V139" t="inlineStr"/>
+      <c r="W139" t="inlineStr"/>
+      <c r="X139" t="inlineStr"/>
+      <c r="Y139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -10106,16 +10674,16 @@
         <v>0</v>
       </c>
       <c r="M140" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N140" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O140" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P140" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q140" t="n">
         <v>54</v>
@@ -10130,6 +10698,10 @@
       </c>
       <c r="T140" t="inlineStr"/>
       <c r="U140" t="inlineStr"/>
+      <c r="V140" t="inlineStr"/>
+      <c r="W140" t="inlineStr"/>
+      <c r="X140" t="inlineStr"/>
+      <c r="Y140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -10175,16 +10747,16 @@
         <v>0</v>
       </c>
       <c r="M141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q141" t="n">
         <v>42</v>
@@ -10199,6 +10771,10 @@
       </c>
       <c r="T141" t="inlineStr"/>
       <c r="U141" t="inlineStr"/>
+      <c r="V141" t="inlineStr"/>
+      <c r="W141" t="inlineStr"/>
+      <c r="X141" t="inlineStr"/>
+      <c r="Y141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -10244,16 +10820,16 @@
         <v>1</v>
       </c>
       <c r="M142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q142" t="n">
         <v>67</v>
@@ -10268,6 +10844,10 @@
       </c>
       <c r="T142" t="inlineStr"/>
       <c r="U142" t="inlineStr"/>
+      <c r="V142" t="inlineStr"/>
+      <c r="W142" t="inlineStr"/>
+      <c r="X142" t="inlineStr"/>
+      <c r="Y142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -10337,6 +10917,10 @@
       </c>
       <c r="T143" t="inlineStr"/>
       <c r="U143" t="inlineStr"/>
+      <c r="V143" t="inlineStr"/>
+      <c r="W143" t="inlineStr"/>
+      <c r="X143" t="inlineStr"/>
+      <c r="Y143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -10406,6 +10990,10 @@
       </c>
       <c r="T144" t="inlineStr"/>
       <c r="U144" t="inlineStr"/>
+      <c r="V144" t="inlineStr"/>
+      <c r="W144" t="inlineStr"/>
+      <c r="X144" t="inlineStr"/>
+      <c r="Y144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -10451,13 +11039,13 @@
         <v>1</v>
       </c>
       <c r="M145" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N145" t="n">
         <v>0</v>
       </c>
       <c r="O145" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P145" t="n">
         <v>0</v>
@@ -10475,6 +11063,594 @@
       </c>
       <c r="T145" t="inlineStr"/>
       <c r="U145" t="inlineStr"/>
+      <c r="V145" t="inlineStr"/>
+      <c r="W145" t="inlineStr"/>
+      <c r="X145" t="inlineStr"/>
+      <c r="Y145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-08-09</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Malmo FF</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Mjallby AIF</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>1</v>
+      </c>
+      <c r="E146" t="n">
+        <v>3</v>
+      </c>
+      <c r="F146" t="n">
+        <v>1342094</v>
+      </c>
+      <c r="G146" t="n">
+        <v>9</v>
+      </c>
+      <c r="H146" t="n">
+        <v>3</v>
+      </c>
+      <c r="I146" t="n">
+        <v>2</v>
+      </c>
+      <c r="J146" t="n">
+        <v>3</v>
+      </c>
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" t="n">
+        <v>0</v>
+      </c>
+      <c r="N146" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" t="n">
+        <v>1</v>
+      </c>
+      <c r="P146" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q146" t="n">
+        <v>54</v>
+      </c>
+      <c r="R146" t="n">
+        <v>46</v>
+      </c>
+      <c r="S146" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="T146" t="inlineStr"/>
+      <c r="U146" t="inlineStr"/>
+      <c r="V146" t="inlineStr"/>
+      <c r="W146" t="inlineStr"/>
+      <c r="X146" t="inlineStr"/>
+      <c r="Y146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-08-09</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Halmstad</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Sirius</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>0</v>
+      </c>
+      <c r="E147" t="n">
+        <v>1</v>
+      </c>
+      <c r="F147" t="n">
+        <v>1342096</v>
+      </c>
+      <c r="G147" t="n">
+        <v>8</v>
+      </c>
+      <c r="H147" t="n">
+        <v>8</v>
+      </c>
+      <c r="I147" t="n">
+        <v>3</v>
+      </c>
+      <c r="J147" t="n">
+        <v>1</v>
+      </c>
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
+      <c r="L147" t="n">
+        <v>0</v>
+      </c>
+      <c r="M147" t="n">
+        <v>0</v>
+      </c>
+      <c r="N147" t="n">
+        <v>0</v>
+      </c>
+      <c r="O147" t="n">
+        <v>0</v>
+      </c>
+      <c r="P147" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q147" t="n">
+        <v>50</v>
+      </c>
+      <c r="R147" t="n">
+        <v>50</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="T147" t="inlineStr"/>
+      <c r="U147" t="inlineStr"/>
+      <c r="V147" t="inlineStr"/>
+      <c r="W147" t="inlineStr"/>
+      <c r="X147" t="inlineStr"/>
+      <c r="Y147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-08-10</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>AIK Stockholm</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Djurgardens IF</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>0</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>1342090</v>
+      </c>
+      <c r="G148" t="n">
+        <v>3</v>
+      </c>
+      <c r="H148" t="n">
+        <v>5</v>
+      </c>
+      <c r="I148" t="n">
+        <v>2</v>
+      </c>
+      <c r="J148" t="n">
+        <v>2</v>
+      </c>
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" t="n">
+        <v>0</v>
+      </c>
+      <c r="M148" t="n">
+        <v>0</v>
+      </c>
+      <c r="N148" t="n">
+        <v>0</v>
+      </c>
+      <c r="O148" t="n">
+        <v>0</v>
+      </c>
+      <c r="P148" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="n">
+        <v>43</v>
+      </c>
+      <c r="R148" t="n">
+        <v>57</v>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="T148" t="inlineStr"/>
+      <c r="U148" t="inlineStr"/>
+      <c r="V148" t="inlineStr"/>
+      <c r="W148" t="inlineStr"/>
+      <c r="X148" t="inlineStr"/>
+      <c r="Y148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-08-10</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Degerfors IF</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>BK Hacken</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>0</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0</v>
+      </c>
+      <c r="F149" t="n">
+        <v>1342097</v>
+      </c>
+      <c r="G149" t="n">
+        <v>4</v>
+      </c>
+      <c r="H149" t="n">
+        <v>7</v>
+      </c>
+      <c r="I149" t="n">
+        <v>3</v>
+      </c>
+      <c r="J149" t="n">
+        <v>2</v>
+      </c>
+      <c r="K149" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" t="n">
+        <v>0</v>
+      </c>
+      <c r="M149" t="n">
+        <v>0</v>
+      </c>
+      <c r="N149" t="n">
+        <v>0</v>
+      </c>
+      <c r="O149" t="n">
+        <v>0</v>
+      </c>
+      <c r="P149" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="n">
+        <v>31</v>
+      </c>
+      <c r="R149" t="n">
+        <v>69</v>
+      </c>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="T149" t="inlineStr"/>
+      <c r="U149" t="inlineStr"/>
+      <c r="V149" t="inlineStr"/>
+      <c r="W149" t="inlineStr"/>
+      <c r="X149" t="inlineStr"/>
+      <c r="Y149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-08-10</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>IFK Norrkoping</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Hammarby FF</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>0</v>
+      </c>
+      <c r="E150" t="n">
+        <v>2</v>
+      </c>
+      <c r="F150" t="n">
+        <v>1342095</v>
+      </c>
+      <c r="G150" t="n">
+        <v>9</v>
+      </c>
+      <c r="H150" t="n">
+        <v>10</v>
+      </c>
+      <c r="I150" t="n">
+        <v>5</v>
+      </c>
+      <c r="J150" t="n">
+        <v>1</v>
+      </c>
+      <c r="K150" t="n">
+        <v>0</v>
+      </c>
+      <c r="L150" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" t="n">
+        <v>0</v>
+      </c>
+      <c r="N150" t="n">
+        <v>0</v>
+      </c>
+      <c r="O150" t="n">
+        <v>0</v>
+      </c>
+      <c r="P150" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q150" t="n">
+        <v>37</v>
+      </c>
+      <c r="R150" t="n">
+        <v>63</v>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="T150" t="inlineStr"/>
+      <c r="U150" t="inlineStr"/>
+      <c r="V150" t="inlineStr"/>
+      <c r="W150" t="inlineStr"/>
+      <c r="X150" t="inlineStr"/>
+      <c r="Y150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-08-10</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Osters IF</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>IF Brommapojkarna</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>1</v>
+      </c>
+      <c r="E151" t="n">
+        <v>1</v>
+      </c>
+      <c r="F151" t="n">
+        <v>1342093</v>
+      </c>
+      <c r="G151" t="n">
+        <v>3</v>
+      </c>
+      <c r="H151" t="n">
+        <v>1</v>
+      </c>
+      <c r="I151" t="n">
+        <v>1</v>
+      </c>
+      <c r="J151" t="n">
+        <v>5</v>
+      </c>
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="n">
+        <v>1</v>
+      </c>
+      <c r="N151" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q151" t="n">
+        <v>39</v>
+      </c>
+      <c r="R151" t="n">
+        <v>61</v>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="T151" t="inlineStr"/>
+      <c r="U151" t="inlineStr"/>
+      <c r="V151" t="inlineStr"/>
+      <c r="W151" t="inlineStr"/>
+      <c r="X151" t="inlineStr"/>
+      <c r="Y151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>IF Elfsborg</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>IFK Varnamo</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>2</v>
+      </c>
+      <c r="E152" t="n">
+        <v>2</v>
+      </c>
+      <c r="F152" t="n">
+        <v>1342091</v>
+      </c>
+      <c r="G152" t="n">
+        <v>8</v>
+      </c>
+      <c r="H152" t="n">
+        <v>3</v>
+      </c>
+      <c r="I152" t="n">
+        <v>1</v>
+      </c>
+      <c r="J152" t="n">
+        <v>0</v>
+      </c>
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="n">
+        <v>1</v>
+      </c>
+      <c r="N152" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="n">
+        <v>1</v>
+      </c>
+      <c r="P152" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q152" t="n">
+        <v>54</v>
+      </c>
+      <c r="R152" t="n">
+        <v>46</v>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="T152" t="inlineStr"/>
+      <c r="U152" t="inlineStr"/>
+      <c r="V152" t="inlineStr"/>
+      <c r="W152" t="inlineStr"/>
+      <c r="X152" t="inlineStr"/>
+      <c r="Y152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Gais</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>IFK Goteborg</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>0</v>
+      </c>
+      <c r="E153" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" t="n">
+        <v>1342092</v>
+      </c>
+      <c r="G153" t="n">
+        <v>12</v>
+      </c>
+      <c r="H153" t="n">
+        <v>2</v>
+      </c>
+      <c r="I153" t="n">
+        <v>4</v>
+      </c>
+      <c r="J153" t="n">
+        <v>4</v>
+      </c>
+      <c r="K153" t="n">
+        <v>0</v>
+      </c>
+      <c r="L153" t="n">
+        <v>0</v>
+      </c>
+      <c r="M153" t="n">
+        <v>0</v>
+      </c>
+      <c r="N153" t="n">
+        <v>1</v>
+      </c>
+      <c r="O153" t="n">
+        <v>0</v>
+      </c>
+      <c r="P153" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" t="n">
+        <v>62</v>
+      </c>
+      <c r="R153" t="n">
+        <v>38</v>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="T153" t="inlineStr"/>
+      <c r="U153" t="inlineStr"/>
+      <c r="V153" t="inlineStr"/>
+      <c r="W153" t="inlineStr"/>
+      <c r="X153" t="inlineStr"/>
+      <c r="Y153" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>